<commit_message>
Inclusão de custos de transporte no orçameto
</commit_message>
<xml_diff>
--- a/PastaDocAdministrativos/Orçamento.xlsx
+++ b/PastaDocAdministrativos/Orçamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\3SIPG-ExemploGit-2024\PastaDocAdministrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54F4E35-3C24-4300-8C34-A83334808C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF91ED59-A9D1-4100-AF6E-25BAE9A580CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,10 +94,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -141,14 +141,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2EA89B41-F4BB-4B02-9DCF-F4BCCA08659A}" name="Table2" displayName="Table2" ref="A2:E8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" dataCellStyle="Currency">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2EA89B41-F4BB-4B02-9DCF-F4BCCA08659A}" name="Table2" displayName="Table2" ref="A2:E8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" dataCellStyle="Currency">
   <autoFilter ref="A2:E8" xr:uid="{2EA89B41-F4BB-4B02-9DCF-F4BCCA08659A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{53C5EF5B-51E3-4C31-99F6-6C6DDF4735E1}" name="Column1" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="2" xr3:uid="{00A8DDF4-EC6A-4E48-9B44-DD945200FB55}" name="Column2" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{09A9D36B-F0C8-4B13-A64D-779CCFC86210}" name="Column3" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{1DB44A0D-1AC1-4B85-8421-4024504F1A49}" name="Column4" dataDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{918E48BB-53D3-4099-A55D-502F67D692B4}" name="Column5" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{53C5EF5B-51E3-4C31-99F6-6C6DDF4735E1}" name="Column1" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="2" xr3:uid="{00A8DDF4-EC6A-4E48-9B44-DD945200FB55}" name="Column2" dataDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{09A9D36B-F0C8-4B13-A64D-779CCFC86210}" name="Column3" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{1DB44A0D-1AC1-4B85-8421-4024504F1A49}" name="Column4" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{918E48BB-53D3-4099-A55D-502F67D692B4}" name="Column5" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -420,7 +420,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,13 +429,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -455,104 +455,104 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1900</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1900</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1900</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1900</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1900</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2000</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2000</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2000</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2000</v>
+      <c r="A4" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>2100</v>
       </c>
-      <c r="B5" s="3">
-        <v>2000</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2000</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="B5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E5" s="2">
         <v>2000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>2200</v>
       </c>
-      <c r="B6" s="3">
-        <v>2000</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2000</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E6" s="2">
         <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>2300</v>
       </c>
-      <c r="B7" s="3">
-        <v>2000</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2000</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="B7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="2">
         <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>2400</v>
       </c>
-      <c r="B8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="B8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E8" s="2">
         <v>2000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Resolvido valores incorretos na doc de orçamentos
</commit_message>
<xml_diff>
--- a/PastaDocAdministrativos/Orçamento.xlsx
+++ b/PastaDocAdministrativos/Orçamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Desktop\3SIPG-ExemploGit-2024\PastaDocAdministrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF91ED59-A9D1-4100-AF6E-25BAE9A580CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D08448E-1B4A-4A2D-890A-CD2F773135CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,16 +476,16 @@
         <v>2000</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="2">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>